<commit_message>
Latest aggregated outputs - 14 Feb 2024
</commit_message>
<xml_diff>
--- a/gaza_overall/inputs/gaza_overall_parameters.xlsx
+++ b/gaza_overall/inputs/gaza_overall_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\gaza\gaza_overall\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D52C6F2-CC35-46D1-BCFB-9F74DB708AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E4300B-EB50-44EB-94F9-1D8927DB8C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="92">
   <si>
     <t>parameter</t>
   </si>
@@ -186,12 +186,6 @@
   </si>
   <si>
     <t>Shigella dysenteriae type 1</t>
-  </si>
-  <si>
-    <t>runs</t>
-  </si>
-  <si>
-    <t>number of bootstrap runs</t>
   </si>
   <si>
     <t>polio - wildtype</t>
@@ -763,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583212BB-FE43-40DF-83EF-3CBB0F7B7681}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -794,65 +788,59 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="D4" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="9">
-        <v>100</v>
-      </c>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -878,24 +866,18 @@
       <c r="C10" s="7"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="9"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="expression" dxfId="2" priority="5">
       <formula>#REF!="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="expression" dxfId="1" priority="6">
       <formula>#REF!="Y"</formula>
     </cfRule>
@@ -911,7 +893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83D5307-C8FB-4E01-831D-6A382C74EA7D}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -923,21 +905,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>72</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="14">
         <v>2959</v>
@@ -951,7 +933,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="14">
         <v>32545</v>
@@ -965,7 +947,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="14">
         <v>136078</v>
@@ -979,7 +961,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="14">
         <v>145276</v>
@@ -993,7 +975,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="14">
         <v>141660</v>
@@ -1007,7 +989,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B7" s="14">
         <v>120553</v>
@@ -1021,7 +1003,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" s="14">
         <v>98073</v>
@@ -1035,7 +1017,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9" s="14">
         <v>97192</v>
@@ -1049,7 +1031,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10" s="14">
         <v>87562</v>
@@ -1063,7 +1045,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" s="14">
         <v>64156</v>
@@ -1077,7 +1059,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B12" s="14">
         <v>49109</v>
@@ -1091,7 +1073,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B13" s="14">
         <v>41317</v>
@@ -1105,7 +1087,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B14" s="14">
         <v>31260</v>
@@ -1119,7 +1101,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B15" s="14">
         <v>28753</v>
@@ -1133,7 +1115,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B16" s="14">
         <v>20588</v>
@@ -1147,7 +1129,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B17" s="14">
         <v>13323</v>
@@ -1161,7 +1143,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" s="14">
         <v>9282</v>
@@ -1175,7 +1157,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B19" s="14">
         <v>4934</v>
@@ -1189,7 +1171,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B20" s="14">
         <v>3293</v>
@@ -1215,7 +1197,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,19 +1215,19 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G1" s="4"/>
     </row>
@@ -1260,10 +1242,10 @@
         <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -1281,10 +1263,10 @@
         <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>5</v>
@@ -1302,10 +1284,10 @@
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>6</v>
@@ -1323,7 +1305,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
@@ -1335,19 +1317,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>6</v>
@@ -1356,19 +1338,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>6</v>
@@ -1386,7 +1368,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>19</v>
@@ -1407,7 +1389,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>19</v>
@@ -1428,7 +1410,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>19</v>
@@ -1449,7 +1431,7 @@
         <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>19</v>
@@ -1470,7 +1452,7 @@
         <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>19</v>
@@ -1491,10 +1473,10 @@
         <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>6</v>
@@ -1512,10 +1494,10 @@
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>6</v>
@@ -1533,7 +1515,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>19</v>
@@ -1554,7 +1536,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>19</v>
@@ -1575,7 +1557,7 @@
         <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>19</v>
@@ -1596,10 +1578,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>6</v>
@@ -1617,7 +1599,7 @@
         <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>19</v>
@@ -1638,7 +1620,7 @@
         <v>21</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>19</v>

</xml_diff>